<commit_message>
Se concluye el proyecto
</commit_message>
<xml_diff>
--- a/Regresion-Interpolacion.xlsx
+++ b/Regresion-Interpolacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unicaucaeduco-my.sharepoint.com/personal/juanoa_unicauca_edu_co/Documents/UNIVERSIDAD/Semestre2021.1/Analisis Numerico/Parcial-2-2021-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="784" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{78E87767-3BD2-4757-9A95-4F9CCCFD6722}"/>
+  <xr:revisionPtr revIDLastSave="970" documentId="11_9248B46DC1CBB2E3ED7FF6F9903E8C1851038383" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{55C37B29-8862-4E5B-8EA8-170A430C177A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -150,11 +150,44 @@
   <si>
     <t>f(0,08)</t>
   </si>
+  <si>
+    <t>POLINOMIO DE INTERPOLACION</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POLINOMIO DE INTERPOLACION </t>
+  </si>
+  <si>
+    <t xml:space="preserve">               =</t>
+  </si>
+  <si>
+    <t>CALCULO DEL ERROR</t>
+  </si>
+  <si>
+    <t>Caso 1</t>
+  </si>
+  <si>
+    <t>Caso 2</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">f = </t>
+  </si>
+  <si>
+    <t>ERROR DE INTERPOLACION</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="171" formatCode="0.0000000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -164,7 +197,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,8 +252,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -558,11 +603,109 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -601,15 +744,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -624,9 +758,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -644,6 +775,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,6 +841,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF0000"/>
+      <color rgb="FF00FFFF"/>
       <color rgb="FFFF6600"/>
       <color rgb="FFCC99FF"/>
       <color rgb="FF68D000"/>
@@ -4845,6 +5036,94 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1100666</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>84667</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>633717</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>45558</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF55EDED-FD42-4CDF-B9B8-BE0A1093F274}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10244666" y="6043084"/>
+          <a:ext cx="5973009" cy="352474"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>751417</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>137583</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>48496</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>98474</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EE54BDC-9A46-46AF-B2C7-0830A887F33C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="751417" y="8424333"/>
+          <a:ext cx="6239746" cy="352474"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5456,8 +5735,8 @@
       </c>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
+      <c r="C57" s="42"/>
+      <c r="D57" s="42"/>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C58" s="2"/>
@@ -5498,20 +5777,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B75BD078-DD7C-4543-9D69-F110EEC51D30}">
-  <dimension ref="B3:M43"/>
+  <dimension ref="B3:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
@@ -5607,28 +5888,28 @@
       <c r="C12" s="10"/>
       <c r="D12" s="10"/>
     </row>
-    <row r="18" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="19" t="s">
+    <row r="18" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F19" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="35"/>
-      <c r="H19" s="19" t="s">
+      <c r="G19" s="44"/>
+      <c r="H19" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="I19" s="20"/>
-      <c r="J19" s="19" t="s">
+      <c r="I19" s="45"/>
+      <c r="J19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="K19" s="20"/>
-      <c r="L19" s="19" t="s">
+      <c r="K19" s="45"/>
+      <c r="L19" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="M19" s="20"/>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M19" s="45"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F20" s="12"/>
-      <c r="G20" s="36"/>
+      <c r="G20" s="32"/>
       <c r="H20" s="12"/>
       <c r="I20" s="13"/>
       <c r="J20" s="12"/>
@@ -5636,11 +5917,11 @@
       <c r="L20" s="12"/>
       <c r="M20" s="13"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F21" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="30">
+      <c r="G21" s="27">
         <f>(D5-D4)/(C5-C4)</f>
         <v>2.6366479999999992</v>
       </c>
@@ -5666,12 +5947,12 @@
         <v>1.4986666666665327</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F22" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G22" s="30">
-        <f>(D6-D5)/(C6-C5)</f>
+      <c r="G22" s="27">
+        <f t="shared" ref="G21:G26" si="0">(D6-D5)/(C6-C5)</f>
         <v>1.95932</v>
       </c>
       <c r="H22" s="14" t="s">
@@ -5681,27 +5962,27 @@
         <f>(G23-G22)/(C7-C5)</f>
         <v>-5.9824999999999999</v>
       </c>
-      <c r="J22" s="21" t="s">
+      <c r="J22" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="K22" s="22">
+      <c r="K22" s="19">
         <f>(I23-I22)/(C8-C5)</f>
         <v>5.5715999999999246</v>
       </c>
-      <c r="L22" s="21" t="s">
+      <c r="L22" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="M22" s="22">
+      <c r="M22" s="19">
         <f>(K23-K22)/(C9-C5)</f>
         <v>0.64533333333469667</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F23" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G23" s="30">
-        <f>(D7-D6)/(C7-C6)</f>
+      <c r="G23" s="27">
+        <f t="shared" si="0"/>
         <v>1.36107</v>
       </c>
       <c r="H23" s="14" t="s">
@@ -5726,12 +6007,12 @@
         <v>-0.14533333333434761</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F24" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G24" s="30">
-        <f>(D8-D7)/(C8-C7)</f>
+      <c r="G24" s="27">
+        <f t="shared" si="0"/>
         <v>0.84639399999999887</v>
       </c>
       <c r="H24" s="14" t="s">
@@ -5741,25 +6022,25 @@
         <f>(G25-G24)/(C9-C7)</f>
         <v>-4.2916599999999816</v>
       </c>
-      <c r="J24" s="31" t="s">
+      <c r="J24" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="K24" s="32">
+      <c r="K24" s="29">
         <f>(I25-I24)/(C10-C7)</f>
         <v>5.6715999999999944</v>
       </c>
       <c r="L24" s="14"/>
       <c r="M24" s="15"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F25" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="G25" s="30">
-        <f>(D9-D8)/(C9-C8)</f>
+      <c r="G25" s="27">
+        <f t="shared" si="0"/>
         <v>0.41722800000000071</v>
       </c>
-      <c r="H25" s="21" t="s">
+      <c r="H25" s="18" t="s">
         <v>24</v>
       </c>
       <c r="I25" s="15">
@@ -5768,25 +6049,25 @@
       </c>
       <c r="J25" s="14"/>
       <c r="K25" s="15"/>
-      <c r="L25" s="33"/>
-      <c r="M25" s="34"/>
-    </row>
-    <row r="26" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L25" s="30"/>
+      <c r="M25" s="31"/>
+    </row>
+    <row r="26" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F26" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="G26" s="28">
-        <f>(D10-D9)/(C10-C9)</f>
+      <c r="G26" s="25">
+        <f t="shared" si="0"/>
         <v>7.3136000000002546E-2</v>
       </c>
       <c r="H26" s="16"/>
-      <c r="I26" s="29"/>
+      <c r="I26" s="26"/>
       <c r="J26" s="16"/>
-      <c r="K26" s="23"/>
+      <c r="K26" s="20"/>
       <c r="L26" s="16"/>
-      <c r="M26" s="23"/>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M26" s="20"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>37</v>
       </c>
@@ -5794,8 +6075,8 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="28" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>36</v>
       </c>
@@ -5805,23 +6086,30 @@
       <c r="D29" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F29" s="39" t="s">
+      <c r="F29" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="G29" s="39" t="s">
+      <c r="G29" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="H29" s="39" t="s">
+      <c r="H29" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="I29" s="39" t="s">
+      <c r="I29" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="K29" s="27" t="s">
+      <c r="K29" s="24" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="L29" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="M29" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="N29" s="40"/>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30">
         <f>$C$27-C30</f>
         <v>0.08</v>
@@ -5832,16 +6120,16 @@
       <c r="D30" s="6">
         <v>1</v>
       </c>
-      <c r="F30" s="40">
+      <c r="F30" s="36">
         <v>1</v>
       </c>
-      <c r="G30" s="40">
+      <c r="G30" s="36">
         <v>2.6366480000000001</v>
       </c>
-      <c r="H30" s="40">
+      <c r="H30" s="36">
         <v>-6.7732799999999997</v>
       </c>
-      <c r="I30" s="40">
+      <c r="I30" s="36">
         <v>5.2718666699999996</v>
       </c>
       <c r="K30">
@@ -5849,9 +6137,9 @@
         <v>1.1944229183998401</v>
       </c>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31">
-        <f t="shared" ref="B31:B33" si="0">$C$27-C31</f>
+        <f>$C$27-C31</f>
         <v>0.03</v>
       </c>
       <c r="C31" s="6">
@@ -5860,14 +6148,14 @@
       <c r="D31" s="6">
         <v>1.1318324</v>
       </c>
-      <c r="F31" s="41"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="41"/>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F31" s="37"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="37"/>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32">
-        <f t="shared" si="0"/>
+        <f>$C$27-C32</f>
         <v>-2.0000000000000004E-2</v>
       </c>
       <c r="C32" s="6">
@@ -5876,55 +6164,75 @@
       <c r="D32" s="6">
         <v>1.2297984</v>
       </c>
-      <c r="F32" s="41"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="41"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="37"/>
       <c r="J32" s="11"/>
       <c r="K32" s="11"/>
       <c r="L32" s="11"/>
       <c r="M32" s="11"/>
     </row>
-    <row r="33" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <f>$C$27-C33</f>
+        <v>-6.9999999999999993E-2</v>
+      </c>
       <c r="C33" s="6">
         <v>0.15</v>
       </c>
       <c r="D33" s="6">
         <v>1.2978518999999999</v>
       </c>
-      <c r="F33" s="42"/>
-      <c r="G33" s="42"/>
-      <c r="H33" s="42"/>
-      <c r="I33" s="42"/>
-    </row>
-    <row r="35" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+    </row>
+    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C34" s="46">
+        <v>0.2</v>
+      </c>
+      <c r="D34" s="47">
+        <v>1.3401715999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="37" t="s">
+      <c r="C36" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="D36" s="37" t="s">
+      <c r="D36" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="F36" s="38" t="s">
+      <c r="F36" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="G36" s="38" t="s">
+      <c r="G36" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="H36" s="38" t="s">
+      <c r="H36" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="I36" s="38" t="s">
+      <c r="I36" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="K36" s="38" t="s">
+      <c r="K36" s="34" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="L36" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="M36" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="N36" s="40"/>
+      <c r="O36" s="40"/>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37">
         <f>$C$27-C37</f>
         <v>0.03</v>
@@ -5935,16 +6243,16 @@
       <c r="D37" s="6">
         <v>1.1318324</v>
       </c>
-      <c r="F37" s="26">
+      <c r="F37" s="23">
         <v>1.1318324</v>
       </c>
-      <c r="G37" s="26">
+      <c r="G37" s="23">
         <v>1.95932</v>
       </c>
-      <c r="H37" s="26">
+      <c r="H37" s="23">
         <v>-5.9824999999999999</v>
       </c>
-      <c r="I37" s="26">
+      <c r="I37" s="23">
         <v>5.5716000000000001</v>
       </c>
       <c r="K37">
@@ -5952,7 +6260,7 @@
         <v>1.1944355071999999</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B38">
         <f>$C$27-C38</f>
         <v>-2.0000000000000004E-2</v>
@@ -5963,14 +6271,14 @@
       <c r="D38" s="6">
         <v>1.2297984</v>
       </c>
-      <c r="F38" s="24"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="24"/>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B39">
-        <f t="shared" ref="B38:B39" si="1">$C$27-C39</f>
+        <f t="shared" ref="B38:B40" si="1">$C$27-C39</f>
         <v>-6.9999999999999993E-2</v>
       </c>
       <c r="C39" s="6">
@@ -5979,37 +6287,201 @@
       <c r="D39" s="6">
         <v>1.2978518999999999</v>
       </c>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
-      <c r="I39" s="24"/>
-    </row>
-    <row r="40" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
+    </row>
+    <row r="40" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <f t="shared" si="1"/>
+        <v>-0.12000000000000001</v>
+      </c>
       <c r="C40" s="6">
         <v>0.2</v>
       </c>
       <c r="D40" s="6">
         <v>1.3401715999999999</v>
       </c>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="25"/>
-      <c r="I40" s="25"/>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="22"/>
+    </row>
+    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C41" s="46">
+        <v>0.25</v>
+      </c>
+      <c r="D41" s="47">
+        <v>1.3646898000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C43" s="10"/>
+    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C43" s="10" t="s">
+        <v>43</v>
+      </c>
       <c r="D43" s="10"/>
     </row>
+    <row r="45" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J45" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L46" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="M46" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="N46" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="O46" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="P46" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="R46" s="60" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B47" s="63" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" s="64"/>
+      <c r="L47" s="36">
+        <v>1</v>
+      </c>
+      <c r="M47" s="36">
+        <v>2.6366480000000001</v>
+      </c>
+      <c r="N47" s="36">
+        <v>-6.7732799999999997</v>
+      </c>
+      <c r="O47" s="51">
+        <v>5.2718666699999996</v>
+      </c>
+      <c r="P47" s="21">
+        <v>1.4986667</v>
+      </c>
+      <c r="R47">
+        <f>L47+M47*B30+N47*B30*B31+O47*B30*B31*B32+P47*B30*B31*B32*B33</f>
+        <v>1.194427953919952</v>
+      </c>
+    </row>
+    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B48" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C48" s="47">
+        <f>($R$47)*(C27-C30)*(C27-C31)*(C27-C32)*(C27-C33)</f>
+        <v>4.0132779251710393E-6</v>
+      </c>
+      <c r="L48" s="37"/>
+      <c r="M48" s="37"/>
+      <c r="N48" s="37"/>
+      <c r="O48" s="52"/>
+      <c r="P48" s="21"/>
+    </row>
+    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B49" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49" s="47">
+        <f>($R$47)*(C27-C37)*(C27-C38)*(C27-C39)*(C27-C40)</f>
+        <v>-6.0199168877565602E-6</v>
+      </c>
+      <c r="L49" s="37"/>
+      <c r="M49" s="37"/>
+      <c r="N49" s="37"/>
+      <c r="O49" s="52"/>
+      <c r="P49" s="21"/>
+    </row>
+    <row r="50" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L50" s="38"/>
+      <c r="M50" s="38"/>
+      <c r="N50" s="38"/>
+      <c r="O50" s="53"/>
+      <c r="P50" s="22"/>
+    </row>
+    <row r="51" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E52" s="62"/>
+      <c r="L52" s="57" t="s">
+        <v>32</v>
+      </c>
+      <c r="M52" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="N52" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="O52" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="P52" s="59" t="s">
+        <v>46</v>
+      </c>
+      <c r="R52" s="61" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="L53" s="23">
+        <v>1.1318324</v>
+      </c>
+      <c r="M53" s="23">
+        <v>1.95932</v>
+      </c>
+      <c r="N53" s="23">
+        <v>-5.9824999999999999</v>
+      </c>
+      <c r="O53" s="48">
+        <v>5.5716000000000001</v>
+      </c>
+      <c r="P53" s="21">
+        <v>0.6453333</v>
+      </c>
+      <c r="R53">
+        <f>L53+M53*B37+N53*B37*B38+O53*B37*B38*B39+P53*B37*B38*B39*B40</f>
+        <v>1.194432254720168</v>
+      </c>
+    </row>
+    <row r="54" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="L54" s="21"/>
+      <c r="M54" s="21"/>
+      <c r="N54" s="21"/>
+      <c r="O54" s="49"/>
+      <c r="P54" s="21"/>
+    </row>
+    <row r="55" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="L55" s="21"/>
+      <c r="M55" s="21"/>
+      <c r="N55" s="21"/>
+      <c r="O55" s="49"/>
+      <c r="P55" s="21"/>
+    </row>
+    <row r="56" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L56" s="22"/>
+      <c r="M56" s="22"/>
+      <c r="N56" s="22"/>
+      <c r="O56" s="50"/>
+      <c r="P56" s="22"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="H19:I19"/>
     <mergeCell ref="J19:K19"/>
     <mergeCell ref="L19:M19"/>
+    <mergeCell ref="B47:C47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>